<commit_message>
- No hay nada nuevo, solo estuve probando xd
</commit_message>
<xml_diff>
--- a/src/main/resources/test.xlsx
+++ b/src/main/resources/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="router" sheetId="1" state="visible" r:id="rId2"/>
@@ -232,7 +232,7 @@
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -332,8 +332,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -343,13 +343,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -389,32 +389,32 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="n">
-        <v>4</v>
+      <c r="A6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2</v>
@@ -422,10 +422,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -433,30 +433,46 @@
         <v>4</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B15" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B14" s="0" t="n">
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B16" s="0" t="n">
         <v>5</v>
       </c>
     </row>
@@ -465,8 +481,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -478,11 +494,11 @@
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K23" activeCellId="0" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -637,8 +653,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>